<commit_message>
controlMode support - client
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Dev\robot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{00A252C9-C703-4B6D-BB08-AF5F6B6A36FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5035B04-FB7E-4BD5-A161-0CC85B5ABA01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D60E77E5-5F66-4C84-9492-2E321D3A95AE}"/>
   </bookViews>
@@ -32,12 +32,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>Distance (cm)</t>
-  </si>
-  <si>
-    <t>error</t>
   </si>
   <si>
     <r>
@@ -115,9 +112,6 @@
     <t>Obstacle straight on</t>
   </si>
   <si>
-    <t>Better pattern. Just going to optimize for 8cm</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">n </t>
     </r>
@@ -139,10 +133,19 @@
     <t>Average error = -6.406%</t>
   </si>
   <si>
-    <t>fudged</t>
+    <t>Measured (cm)</t>
   </si>
   <si>
-    <t>Measured (cm)</t>
+    <t>Fudged Distance (cm)</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>Eerror</t>
+  </si>
+  <si>
+    <t>Better pattern. But I'll just optimize for 8cm--a close distance where accuracy is more critical.</t>
   </si>
 </sst>
 </file>
@@ -2481,25 +2484,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2697B148-6447-4D65-8A1C-9EDBB5BF5178}">
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="N39" sqref="N39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" customWidth="1"/>
     <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
     <col min="13" max="13" width="82" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -2507,13 +2512,13 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="M3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -2593,13 +2598,13 @@
         <v>0</v>
       </c>
       <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" t="s">
         <v>11</v>
       </c>
-      <c r="C18" t="s">
-        <v>1</v>
-      </c>
       <c r="M18" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -2614,7 +2619,7 @@
         <v>-9.9999999999999978E-2</v>
       </c>
       <c r="M19" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -2694,16 +2699,16 @@
         <v>0</v>
       </c>
       <c r="B33" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C33" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D33" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M33" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
@@ -2722,7 +2727,7 @@
         <v>8.1198399999999999</v>
       </c>
       <c r="M34" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
@@ -2741,7 +2746,7 @@
         <v>7.9061600000000007</v>
       </c>
       <c r="M35" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>